<commit_message>
Profile and historical data for SIMP Map
</commit_message>
<xml_diff>
--- a/data/Profiles.xlsx
+++ b/data/Profiles.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jac\Documents\BSc Computing Year 4 Pt2\Dissertation\RTest\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Scotland\dc1\FS2_Home\u207109\Personal\UHI Bits\Dissertation\Practical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7CE56B-E43C-4D1C-A1EA-FFAC2FE7C510}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2505" windowWidth="15375" windowHeight="7875" xr2:uid="{E269F835-FF74-4934-9ABD-755BA1AA99D1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,7 +233,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,12 +596,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0316F37A-B33F-4098-8660-E117966C5E83}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -876,38 +873,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/aberdeen-city-council-profile.html" xr:uid="{C260FB10-88EB-4F4B-ACB5-89122DFEFB64}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/aberdeenshire-council-profile.html" xr:uid="{2AA12048-CFB7-45F3-B5C0-89BC8CD1A6F7}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/angus-council-profile.html" xr:uid="{E8741F28-2F96-41CC-974F-85A195419099}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/argyll-and-bute-council-profile.html" xr:uid="{8895466E-31F5-4EBE-B54D-1A0ACC537173}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/city-of-edinburgh-council-profile.html" xr:uid="{C5D67AA2-0A4C-4D2C-BC99-2E03F54CB606}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/clackmannanshire-council-profile.html" xr:uid="{51ED3088-1A3A-462E-BA80-CF6A2AA11E29}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/dumfries-and-galloway-council-profile.html" xr:uid="{6B3F304F-2790-4B6C-8AEA-50056308D976}"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/dundee-city-council-profile.html" xr:uid="{67352D02-76DA-41CA-82EF-6C48FFC5D7D0}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-ayrshire-council-profile.html" xr:uid="{9951C187-2E24-4938-9CFA-FC274E072F0A}"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-dunbartonshire-council-profile.html" xr:uid="{D3E53CA7-BA3B-4645-B0FD-B2AE2784BA2F}"/>
-    <hyperlink ref="B12" r:id="rId11" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-lothian-council-profile.html" xr:uid="{5AEFB911-7F96-495C-999A-A6EF2DA5369F}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-renfrewshire-council-profile.html" xr:uid="{F78B6B7A-4608-44BA-A0C2-024AF0CAC721}"/>
-    <hyperlink ref="B14" r:id="rId13" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/falkirk-council-profile.html" xr:uid="{09EB4444-430B-4D4E-8CB1-DB7A71CA6621}"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/fife-council-profile.html" xr:uid="{519540C3-BBFE-4353-9BE7-9B914E7FA2BB}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/glasgow-city-council-profile.html" xr:uid="{467D02E8-9356-4EF3-ACE9-2EB4B435B549}"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/highland-council-profile.html" xr:uid="{EC75107A-8397-4EEF-96A3-A6D69510B004}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/inverclyde-council-profile.html" xr:uid="{49D6874E-6E26-4F95-99C7-BA55D7979452}"/>
-    <hyperlink ref="B19" r:id="rId18" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/midlothian-council-profile.html" xr:uid="{06B3EA18-19F3-4012-BE47-1EFC5A8192E7}"/>
-    <hyperlink ref="B20" r:id="rId19" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/moray-council-profile.html" xr:uid="{EA103EBA-E458-4A63-ABE6-DB2B4230AB3E}"/>
-    <hyperlink ref="B21" r:id="rId20" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/na-h-eileanan-siar-council-profile.html" xr:uid="{151CAD40-56D1-4EF4-9798-B251B1B77E3E}"/>
-    <hyperlink ref="B22" r:id="rId21" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/north-ayrshire-council-profile.html" xr:uid="{88A360B7-2D88-41DA-A867-85F6A18CED7E}"/>
-    <hyperlink ref="B23" r:id="rId22" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/north-lanarkshire-council-profile.html" xr:uid="{80CB51CF-8C1B-4A5E-A99E-7BCFBBB1B747}"/>
-    <hyperlink ref="B24" r:id="rId23" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/orkney-islands-council-profile.html" xr:uid="{02DD9D4A-5E8C-46A0-B19C-D82AD6503608}"/>
-    <hyperlink ref="B25" r:id="rId24" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/perth-and-kinross-council-profile.html" xr:uid="{2AABA29A-9602-4F28-BB83-6022C828FB0B}"/>
-    <hyperlink ref="B26" r:id="rId25" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/renfrewshire-council-profile.html" xr:uid="{1B842C28-D340-4C2F-A252-029E82C24DDB}"/>
-    <hyperlink ref="B27" r:id="rId26" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/scottish-borders-council-profile.html" xr:uid="{0913135D-A05F-4FB1-99A2-2EC46531694E}"/>
-    <hyperlink ref="B28" r:id="rId27" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/shetland-islands-council-profile.html" xr:uid="{2053F8CF-F3D2-46BD-B5DE-158B6FE58D78}"/>
-    <hyperlink ref="B29" r:id="rId28" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/south-ayrshire-council-profile.html" xr:uid="{FEA47833-C3CF-44FA-8CFC-AA46A690FB81}"/>
-    <hyperlink ref="B30" r:id="rId29" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/south-lanarkshire-council-profile.html" xr:uid="{FEFAA32F-286F-4B8D-8CAB-1113EB06B1A9}"/>
-    <hyperlink ref="B31" r:id="rId30" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/stirling-council-profile.html" xr:uid="{50C4AF4E-F819-4D04-A36E-1702F94F6AF6}"/>
-    <hyperlink ref="B32" r:id="rId31" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/west-dunbartonshire-council-profile.html" xr:uid="{2439C635-B667-4588-B8EF-B77504319C1E}"/>
-    <hyperlink ref="B33" r:id="rId32" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/west-lothian-council-profile.html" xr:uid="{6FA25448-0A5A-4516-946D-63E7DA7509F9}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/aberdeen-city-council-profile.html"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/aberdeenshire-council-profile.html"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/angus-council-profile.html"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/argyll-and-bute-council-profile.html"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/city-of-edinburgh-council-profile.html"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/clackmannanshire-council-profile.html"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/dumfries-and-galloway-council-profile.html"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/dundee-city-council-profile.html"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-ayrshire-council-profile.html"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-dunbartonshire-council-profile.html"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-lothian-council-profile.html"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/east-renfrewshire-council-profile.html"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/falkirk-council-profile.html"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/fife-council-profile.html"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/glasgow-city-council-profile.html"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/highland-council-profile.html"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/inverclyde-council-profile.html"/>
+    <hyperlink ref="B19" r:id="rId18" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/midlothian-council-profile.html"/>
+    <hyperlink ref="B20" r:id="rId19" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/moray-council-profile.html"/>
+    <hyperlink ref="B21" r:id="rId20" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/na-h-eileanan-siar-council-profile.html"/>
+    <hyperlink ref="B22" r:id="rId21" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/north-ayrshire-council-profile.html"/>
+    <hyperlink ref="B23" r:id="rId22" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/north-lanarkshire-council-profile.html"/>
+    <hyperlink ref="B24" r:id="rId23" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/orkney-islands-council-profile.html"/>
+    <hyperlink ref="B25" r:id="rId24" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/perth-and-kinross-council-profile.html"/>
+    <hyperlink ref="B26" r:id="rId25" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/renfrewshire-council-profile.html"/>
+    <hyperlink ref="B27" r:id="rId26" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/scottish-borders-council-profile.html"/>
+    <hyperlink ref="B28" r:id="rId27" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/shetland-islands-council-profile.html"/>
+    <hyperlink ref="B29" r:id="rId28" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/south-ayrshire-council-profile.html"/>
+    <hyperlink ref="B30" r:id="rId29" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/south-lanarkshire-council-profile.html"/>
+    <hyperlink ref="B31" r:id="rId30" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/stirling-council-profile.html"/>
+    <hyperlink ref="B32" r:id="rId31" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/west-dunbartonshire-council-profile.html"/>
+    <hyperlink ref="B33" r:id="rId32" display="https://www.nrscotland.gov.uk/files/statistics/council-area-data-sheets/west-lothian-council-profile.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>

</xml_diff>